<commit_message>
Made significant corrections in code
</commit_message>
<xml_diff>
--- a/data/2020-01-29.xlsx
+++ b/data/2020-01-29.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -721,7 +721,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -731,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>